<commit_message>
Add video update option
</commit_message>
<xml_diff>
--- a/media/searchdata.xlsx
+++ b/media/searchdata.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A86"/>
+  <dimension ref="A1:A198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A30"/>
@@ -1037,6 +1037,790 @@
         </is>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Emotional Nasheed - Har Ek Janib Udasi Hai - Na Jane Kya Ye Alum Hay- Atiq Ur RehmanEmotional Nasheed - Har Ek Janib Udasi Hai - Na Jane Kya Ye Alum Hay- Atiq Ur Rehman.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>❤ Allah tar rasul ke koto valobashten! 😞 Very Emotional Waz with English and bangla subtitle</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Amazing Drone Footage Of Al Masjid Al Haram - YouTube.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>لا حزن يبقى والقرآن الكريم يتلى الشيخ ياسر الدوسري.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Jore Amin Bola By Mufti Kazi Ibrahim - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>ধুমপান করে নামায পরলে নামায হবে কি-.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>১৭ শ্রেণীর লোক মুসলমান হয়েও জান্নাতে যেতে পারবে না! -শায়খ আহমাদুল্লাহ.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>#مشاري_راشد_العفاسي حب اليتامى - Alafasy Hob Alyatamah - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Bangla Nasheed - Bab Al Raja (Bangla Subtitle) - Muhammad Al Muqit - REMINDER.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>#مشاري_راشد_العفاسي حب اليتامى - Alafasy Hob Alyatamah - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>শুধু আল্লাহকে দেখানোর জন্য কোনো কাজ করেছেন কখনো- মিশারী আল আফাসীর তাকওয়া জাগানিয়া সংগীত.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Facebook_4.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>১৭ শ্রেণীর লোক মুসলমান হয়েও জান্নাতে যেতে পারবে না! -শায়খ আহমাদুল্লাহ.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>১০ শ্রেণীর লোক মারা গেলে শাহাদাতের মর্যাদা পাবে / আলোচক ড আবু বকর মুহাম্মাদ যাকারিয়া হাফিযাহুল্লাহ.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Emotional Nasheed - Har Ek Janib Udasi Hai - Na Jane Kya Ye Alum Hay- Atiq Ur RehmanEmotional Nasheed - Har Ek Janib Udasi Hai - Na Jane Kya Ye Alum Hay- Atiq Ur Rehman.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>❤ Allah tar rasul ke koto valobashten! 😞 Very Emotional Waz with English and bangla subtitle</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Amazing Drone Footage Of Al Masjid Al Haram - YouTube.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>لا حزن يبقى والقرآن الكريم يتلى الشيخ ياسر الدوسري.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Jore Amin Bola By Mufti Kazi Ibrahim - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>ধুমপান করে নামায পরলে নামায হবে কি-.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>১৭ শ্রেণীর লোক মুসলমান হয়েও জান্নাতে যেতে পারবে না! -শায়খ আহমাদুল্লাহ.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>#مشاري_راشد_العفاسي حب اليتامى - Alafasy Hob Alyatamah - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Bangla Nasheed - Bab Al Raja (Bangla Subtitle) - Muhammad Al Muqit - REMINDER.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>#مشاري_راشد_العفاسي حب اليتامى - Alafasy Hob Alyatamah - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>শুধু আল্লাহকে দেখানোর জন্য কোনো কাজ করেছেন কখনো- মিশারী আল আফাসীর তাকওয়া জাগানিয়া সংগীত.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Facebook_4.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>১৭ শ্রেণীর লোক মুসলমান হয়েও জান্নাতে যেতে পারবে না! -শায়খ আহমাদুল্লাহ.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>১০ শ্রেণীর লোক মারা গেলে শাহাদাতের মর্যাদা পাবে / আলোচক ড আবু বকর মুহাম্মাদ যাকারিয়া হাফিযাহুল্লাহ.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Emotional Nasheed - Har Ek Janib Udasi Hai - Na Jane Kya Ye Alum Hay- Atiq Ur RehmanEmotional Nasheed - Har Ek Janib Udasi Hai - Na Jane Kya Ye Alum Hay- Atiq Ur Rehman.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>❤ Allah tar rasul ke koto valobashten! 😞 Very Emotional Waz with English and bangla subtitle</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Amazing Drone Footage Of Al Masjid Al Haram - YouTube.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>لا حزن يبقى والقرآن الكريم يتلى الشيخ ياسر الدوسري.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Jore Amin Bola By Mufti Kazi Ibrahim - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>ধুমপান করে নামায পরলে নামায হবে কি-.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>১৭ শ্রেণীর লোক মুসলমান হয়েও জান্নাতে যেতে পারবে না! -শায়খ আহমাদুল্লাহ.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>#مشاري_راشد_العفاسي حب اليتامى - Alafasy Hob Alyatamah - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Bangla Nasheed - Bab Al Raja (Bangla Subtitle) - Muhammad Al Muqit - REMINDER.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>#مشاري_راشد_العفاسي حب اليتامى - Alafasy Hob Alyatamah - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>শুধু আল্লাহকে দেখানোর জন্য কোনো কাজ করেছেন কখনো- মিশারী আল আফাসীর তাকওয়া জাগানিয়া সংগীত.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Facebook_4.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>১৭ শ্রেণীর লোক মুসলমান হয়েও জান্নাতে যেতে পারবে না! -শায়খ আহমাদুল্লাহ.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>১০ শ্রেণীর লোক মারা গেলে শাহাদাতের মর্যাদা পাবে / আলোচক ড আবু বকর মুহাম্মাদ যাকারিয়া হাফিযাহুল্লাহ.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Emotional Nasheed - Har Ek Janib Udasi Hai - Na Jane Kya Ye Alum Hay- Atiq Ur RehmanEmotional Nasheed - Har Ek Janib Udasi Hai - Na Jane Kya Ye Alum Hay- Atiq Ur Rehman.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>❤ Allah tar rasul ke koto valobashten! 😞 Very Emotional Waz with English and bangla subtitle</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Amazing Drone Footage Of Al Masjid Al Haram - YouTube.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>لا حزن يبقى والقرآن الكريم يتلى الشيخ ياسر الدوسري.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Jore Amin Bola By Mufti Kazi Ibrahim - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>ধুমপান করে নামায পরলে নামায হবে কি-.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>১৭ শ্রেণীর লোক মুসলমান হয়েও জান্নাতে যেতে পারবে না! -শায়খ আহমাদুল্লাহ.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>#مشاري_راشد_العفاسي حب اليتامى - Alafasy Hob Alyatamah - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Bangla Nasheed - Bab Al Raja (Bangla Subtitle) - Muhammad Al Muqit - REMINDER.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>#مشاري_راشد_العفاسي حب اليتامى - Alafasy Hob Alyatamah - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>শুধু আল্লাহকে দেখানোর জন্য কোনো কাজ করেছেন কখনো- মিশারী আল আফাসীর তাকওয়া জাগানিয়া সংগীত.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Facebook_4.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>১৭ শ্রেণীর লোক মুসলমান হয়েও জান্নাতে যেতে পারবে না! -শায়খ আহমাদুল্লাহ.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>১০ শ্রেণীর লোক মারা গেলে শাহাদাতের মর্যাদা পাবে / আলোচক ড আবু বকর মুহাম্মাদ যাকারিয়া হাফিযাহুল্লাহ.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Emotional Nasheed - Har Ek Janib Udasi Hai - Na Jane Kya Ye Alum Hay- Atiq Ur RehmanEmotional Nasheed - Har Ek Janib Udasi Hai - Na Jane Kya Ye Alum Hay- Atiq Ur Rehman.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>❤ Allah tar rasul ke koto valobashten! 😞 Very Emotional Waz with English and bangla subtitle</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Amazing Drone Footage Of Al Masjid Al Haram - YouTube.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>No sadness remains and the Noble Qur’an is recited by Sheikh Yasser Al-Dosari.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Jore Amin Bola By Mufti Kazi Ibrahim - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>If you pray after smoking, what will be the prayers -. Mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>16 class people will not be able to go to paradise even if they are Muslims! -Shaykh Ahmadullah.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>#Mishary_Rashed_Al-Afasy love for orphans - Alafasy Hob Alyatamah - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Bangla Nasheed - Bab Al Raja (Bangla Thipttel) - Muhammad Al Muqit - Reminder.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>#Mishary_Rashed_Al-Afasy love for orphans - Alafasy Hob Alyatamah - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Has he ever done anything just to show Allah - Mishari Al Afasi's Taqwa Jagania Sangeet.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Facebook_4.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>16 class people will not be able to go to paradise even if they are Muslims! -Shaykh Ahmadullah.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>If class 10 people die, they will get the status of martyrdom / Dr. Abu Bakr Muhammad Zakaria Hafizahullah.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Emotional Nasheed - Har Ek Janib Udasi Hai - Na Jane Kya Ye Alum Hay- Atiq Ur RehmanEmotional Nasheed - Har Ek Janib Udasi Hai - Na Jane Kya Ye Alum Hay- Atiq Ur Rehman.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>❤ Allah tar rasul ke koto valobashten! 😞 Very Emotional Waz with English and bangla subtitle</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Amazing Drone Footage Of Al Masjid Al Haram - YouTube.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>No sadness remains and the Noble Qur’an is recited by Sheikh Yasser Al-Dosari.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Jore Amin Bola By Mufti Kazi Ibrahim - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>If you pray after smoking, what will be the prayers -. Mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>16 class people will not be able to go to paradise even if they are Muslims! -Shaykh Ahmadullah.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>#Mishary_Rashed_Al-Afasy love for orphans - Alafasy Hob Alyatamah - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Bangla Nasheed - Bab Al Raja (Bangla Thipttel) - Muhammad Al Muqit - Reminder.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>#Mishary_Rashed_Al-Afasy love for orphans - Alafasy Hob Alyatamah - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Has he ever done anything just to show Allah - Mishari Al Afasi's Taqwa Jagania Sangeet.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Facebook_4.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>16 class people will not be able to go to paradise even if they are Muslims! -Shaykh Ahmadullah.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>If class 10 people die, they will get the status of martyrdom / Dr. Abu Bakr Muhammad Zakaria Hafizahullah.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Emotional Nasheed - Har Ek Janib Udasi Hai - Na Jane Kya Ye Alum Hay- Atiq Ur RehmanEmotional Nasheed - Har Ek Janib Udasi Hai - Na Jane Kya Ye Alum Hay- Atiq Ur Rehman.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>❤ Allah tar rasul ke koto valobashten! 😞 Very Emotional Waz with English and bangla subtitle</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>Amazing Drone Footage Of Al Masjid Al Haram - YouTube.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>No sadness remains and the Noble Qur’an is recited by Sheikh Yasser Al-Dosari.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>Jore Amin Bola By Mufti Kazi Ibrahim - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>If you pray after smoking, what will be the prayers -. Mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>16 class people will not be able to go to paradise even if they are Muslims! -Shaykh Ahmadullah.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>#Mishary_Rashed_Al-Afasy love for orphans - Alafasy Hob Alyatamah - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>Bangla Nasheed - Bab Al Raja (Bangla Thipttel) - Muhammad Al Muqit - Reminder.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>#Mishary_Rashed_Al-Afasy love for orphans - Alafasy Hob Alyatamah - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Has he ever done anything just to show Allah - Mishari Al Afasi's Taqwa Jagania Sangeet.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Facebook_4.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>16 class people will not be able to go to paradise even if they are Muslims! -Shaykh Ahmadullah.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>If class 10 people die, they will get the status of martyrdom / Dr. Abu Bakr Muhammad Zakaria Hafizahullah.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Emotional Nasheed - Har Ek Janib Udasi Hai - Na Jane Kya Ye Alum Hay- Atiq Ur RehmanEmotional Nasheed - Har Ek Janib Udasi Hai - Na Jane Kya Ye Alum Hay- Atiq Ur Rehman.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>❤ Allah tar rasul ke koto valobashten! 😞 Very Emotional Waz with English and bangla subtitle</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Amazing Drone Footage Of Al Masjid Al Haram - YouTube.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>No sadness remains and the Noble Qur’an is recited by Sheikh Yasser Al-Dosari.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>Jore Amin Bola By Mufti Kazi Ibrahim - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>If you pray after smoking, what will be the prayers -. Mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>16 class people will not be able to go to paradise even if they are Muslims! -Shaykh Ahmadullah.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>#Mishary_Rashed_Al-Afasy love for orphans - Alafasy Hob Alyatamah - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>Bangla Nasheed - Bab Al Raja (Bangla Thipttel) - Muhammad Al Muqit - Reminder.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>#Mishary_Rashed_Al-Afasy love for orphans - Alafasy Hob Alyatamah - YouTube.MP4</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>Has he ever done anything just to show Allah - Mishari Al Afasi's Taqwa Jagania Sangeet.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>Facebook_4.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>16 class people will not be able to go to paradise even if they are Muslims! -Shaykh Ahmadullah.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>If class 10 people die, they will get the status of martyrdom / Dr. Abu Bakr Muhammad Zakaria Hafizahullah.mp4</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>